<commit_message>
Upload new versions to parse through later
</commit_message>
<xml_diff>
--- a/plasma_planets3.xlsx
+++ b/plasma_planets3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abbyboehm/code_dev/plasma_torus/cthulhu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7EFAC7-A8E8-0C46-A5DF-70A18AD00A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB37C6EF-5DFB-CD4D-8145-F75C97BF56E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="2020" windowWidth="28040" windowHeight="14280" xr2:uid="{7ED9F1B5-9A57-4146-8E94-26F47B218284}"/>
   </bookViews>
@@ -2475,7 +2475,7 @@
     <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
       <pane xSplit="1" topLeftCell="BU1" activePane="topRight" state="frozen"/>
       <selection activeCell="A84" sqref="A84"/>
-      <selection pane="topRight" activeCell="BZ98" sqref="BZ98"/>
+      <selection pane="topRight" activeCell="CA101" sqref="CA101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>